<commit_message>
data for teenagers, I added clothing and apperal
</commit_message>
<xml_diff>
--- a/analysis/Data for age under 25.xlsx
+++ b/analysis/Data for age under 25.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Categories</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Restaurants</t>
+  </si>
+  <si>
+    <t>Apparel and Clothing</t>
   </si>
 </sst>
 </file>
@@ -363,7 +366,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -434,6 +437,17 @@
         <v>647</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>681</v>
+      </c>
+    </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Perfomed EDA / cleaning on spending and reference data
</commit_message>
<xml_diff>
--- a/analysis/Data for age under 25.xlsx
+++ b/analysis/Data for age under 25.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Categories</t>
   </si>
@@ -43,12 +43,15 @@
   </si>
   <si>
     <t>Restaurants</t>
+  </si>
+  <si>
+    <t>Apparel and Clothing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -82,7 +85,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -359,16 +362,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -379,7 +382,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -390,7 +393,7 @@
         <v>2073</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -401,7 +404,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -412,7 +415,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -423,7 +426,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -434,7 +437,18 @@
         <v>647</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>